<commit_message>
Release v2.1: Implement Daily Global Ranking Strategy (Sharpe 0.47)
</commit_message>
<xml_diff>
--- a/data/fundamental_data.xlsx
+++ b/data/fundamental_data.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I175"/>
+  <dimension ref="A1:J274"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,11 @@
           <t>Shares</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Debt_to_Equity</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -498,6 +503,7 @@
       <c r="I2" t="n">
         <v>5200000000</v>
       </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -525,6 +531,7 @@
       <c r="I3" t="n">
         <v>5200000000</v>
       </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -552,6 +559,7 @@
       <c r="I4" t="n">
         <v>5200000000</v>
       </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -583,6 +591,7 @@
       <c r="I5" t="n">
         <v>5200000000</v>
       </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -614,6 +623,7 @@
       <c r="I6" t="n">
         <v>5200000000</v>
       </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -633,6 +643,7 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -660,6 +671,7 @@
       <c r="I8" t="n">
         <v>435000000</v>
       </c>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -687,6 +699,7 @@
       <c r="I9" t="n">
         <v>435000000</v>
       </c>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -714,6 +727,7 @@
       <c r="I10" t="n">
         <v>435000000</v>
       </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -745,6 +759,7 @@
       <c r="I11" t="n">
         <v>435000000</v>
       </c>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -776,6 +791,7 @@
       <c r="I12" t="n">
         <v>435000000</v>
       </c>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -803,6 +819,7 @@
       <c r="I13" t="n">
         <v>4560000000</v>
       </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -830,6 +847,7 @@
       <c r="I14" t="n">
         <v>4560000000</v>
       </c>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -857,6 +875,7 @@
       <c r="I15" t="n">
         <v>4560000000</v>
       </c>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -888,6 +907,7 @@
       <c r="I16" t="n">
         <v>4560000000</v>
       </c>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -919,6 +939,7 @@
       <c r="I17" t="n">
         <v>4560000000</v>
       </c>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -938,6 +959,7 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -965,6 +987,7 @@
       <c r="I19" t="n">
         <v>998000000</v>
       </c>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -992,6 +1015,7 @@
       <c r="I20" t="n">
         <v>998000000</v>
       </c>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1019,6 +1043,7 @@
       <c r="I21" t="n">
         <v>998000000</v>
       </c>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1050,6 +1075,7 @@
       <c r="I22" t="n">
         <v>998000000</v>
       </c>
+      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1081,6 +1107,7 @@
       <c r="I23" t="n">
         <v>998000000</v>
       </c>
+      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1100,6 +1127,7 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1127,6 +1155,7 @@
       <c r="I25" t="n">
         <v>607200000</v>
       </c>
+      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1154,6 +1183,7 @@
       <c r="I26" t="n">
         <v>607200000</v>
       </c>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1181,6 +1211,7 @@
       <c r="I27" t="n">
         <v>607200000</v>
       </c>
+      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1212,6 +1243,7 @@
       <c r="I28" t="n">
         <v>600000000</v>
       </c>
+      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1243,6 +1275,7 @@
       <c r="I29" t="n">
         <v>600000000</v>
       </c>
+      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1262,6 +1295,7 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1289,6 +1323,7 @@
       <c r="I31" t="n">
         <v>3800000000</v>
       </c>
+      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1316,6 +1351,7 @@
       <c r="I32" t="n">
         <v>3800000000</v>
       </c>
+      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1343,6 +1379,7 @@
       <c r="I33" t="n">
         <v>3800000000</v>
       </c>
+      <c r="J33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1374,6 +1411,7 @@
       <c r="I34" t="n">
         <v>3800000000</v>
       </c>
+      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1405,6 +1443,7 @@
       <c r="I35" t="n">
         <v>3800000000</v>
       </c>
+      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1424,6 +1463,7 @@
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1451,6 +1491,7 @@
       <c r="I37" t="n">
         <v>5862743582</v>
       </c>
+      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1478,6 +1519,7 @@
       <c r="I38" t="n">
         <v>6000000000</v>
       </c>
+      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1505,6 +1547,7 @@
       <c r="I39" t="n">
         <v>5862743582</v>
       </c>
+      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1536,6 +1579,7 @@
       <c r="I40" t="n">
         <v>6000000000</v>
       </c>
+      <c r="J40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1567,6 +1611,7 @@
       <c r="I41" t="n">
         <v>6000000000</v>
       </c>
+      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1594,6 +1639,7 @@
       <c r="I42" t="n">
         <v>6721876000</v>
       </c>
+      <c r="J42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1621,6 +1667,7 @@
       <c r="I43" t="n">
         <v>7000000000</v>
       </c>
+      <c r="J43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1648,6 +1695,7 @@
       <c r="I44" t="n">
         <v>7000000000</v>
       </c>
+      <c r="J44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1679,6 +1727,7 @@
       <c r="I45" t="n">
         <v>6721876000</v>
       </c>
+      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1710,6 +1759,7 @@
       <c r="I46" t="n">
         <v>7000000000</v>
       </c>
+      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1737,6 +1787,7 @@
       <c r="I47" t="n">
         <v>3509100000</v>
       </c>
+      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1764,6 +1815,7 @@
       <c r="I48" t="n">
         <v>3509100000</v>
       </c>
+      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1791,6 +1843,7 @@
       <c r="I49" t="n">
         <v>3509100000</v>
       </c>
+      <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1822,6 +1875,7 @@
       <c r="I50" t="n">
         <v>3509100000</v>
       </c>
+      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1853,6 +1907,7 @@
       <c r="I51" t="n">
         <v>3509100000</v>
       </c>
+      <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1880,6 +1935,7 @@
       <c r="I52" t="n">
         <v>4200000000</v>
       </c>
+      <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1907,6 +1963,7 @@
       <c r="I53" t="n">
         <v>4200000000</v>
       </c>
+      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1934,6 +1991,7 @@
       <c r="I54" t="n">
         <v>4200000000</v>
       </c>
+      <c r="J54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1965,6 +2023,7 @@
       <c r="I55" t="n">
         <v>4200000000</v>
       </c>
+      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1996,6 +2055,7 @@
       <c r="I56" t="n">
         <v>4200000000</v>
       </c>
+      <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2015,6 +2075,7 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2042,6 +2103,7 @@
       <c r="I58" t="n">
         <v>334000000</v>
       </c>
+      <c r="J58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2069,6 +2131,7 @@
       <c r="I59" t="n">
         <v>334000000</v>
       </c>
+      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2096,6 +2159,7 @@
       <c r="I60" t="n">
         <v>334000000</v>
       </c>
+      <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2127,6 +2191,7 @@
       <c r="I61" t="n">
         <v>334000000</v>
       </c>
+      <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2158,6 +2223,7 @@
       <c r="I62" t="n">
         <v>334000000</v>
       </c>
+      <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2177,6 +2243,7 @@
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2204,6 +2271,7 @@
       <c r="I64" t="n">
         <v>7037925825</v>
       </c>
+      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2231,6 +2299,7 @@
       <c r="I65" t="n">
         <v>8430000000</v>
       </c>
+      <c r="J65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2258,6 +2327,7 @@
       <c r="I66" t="n">
         <v>8430000000</v>
       </c>
+      <c r="J66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2287,6 +2357,7 @@
       <c r="I67" t="n">
         <v>8430000000</v>
       </c>
+      <c r="J67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2316,6 +2387,7 @@
       <c r="I68" t="n">
         <v>8430000000</v>
       </c>
+      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2335,6 +2407,7 @@
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2362,6 +2435,7 @@
       <c r="I70" t="n">
         <v>25000000000</v>
       </c>
+      <c r="J70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2389,6 +2463,7 @@
       <c r="I71" t="n">
         <v>25000000000</v>
       </c>
+      <c r="J71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2416,6 +2491,7 @@
       <c r="I72" t="n">
         <v>25000000000</v>
       </c>
+      <c r="J72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2447,6 +2523,7 @@
       <c r="I73" t="n">
         <v>25000000000</v>
       </c>
+      <c r="J73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2478,6 +2555,7 @@
       <c r="I74" t="n">
         <v>25000000000</v>
       </c>
+      <c r="J74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2497,6 +2575,7 @@
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2524,6 +2603,7 @@
       <c r="I76" t="n">
         <v>2535898050</v>
       </c>
+      <c r="J76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2551,6 +2631,7 @@
       <c r="I77" t="n">
         <v>2535898050</v>
       </c>
+      <c r="J77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2578,6 +2659,7 @@
       <c r="I78" t="n">
         <v>2535898050</v>
       </c>
+      <c r="J78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2609,6 +2691,7 @@
       <c r="I79" t="n">
         <v>2535898050</v>
       </c>
+      <c r="J79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2640,6 +2723,7 @@
       <c r="I80" t="n">
         <v>2535898050</v>
       </c>
+      <c r="J80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2659,6 +2743,7 @@
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2686,6 +2771,7 @@
       <c r="I82" t="n">
         <v>1258279845</v>
       </c>
+      <c r="J82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2713,6 +2799,7 @@
       <c r="I83" t="n">
         <v>1258279845</v>
       </c>
+      <c r="J83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2740,6 +2827,7 @@
       <c r="I84" t="n">
         <v>1258279845</v>
       </c>
+      <c r="J84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2769,6 +2857,7 @@
       <c r="I85" t="n">
         <v>1258279845</v>
       </c>
+      <c r="J85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2798,6 +2887,7 @@
       <c r="I86" t="n">
         <v>1258279845</v>
       </c>
+      <c r="J86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2817,6 +2907,7 @@
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2844,6 +2935,7 @@
       <c r="I88" t="n">
         <v>1140000000</v>
       </c>
+      <c r="J88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2871,6 +2963,7 @@
       <c r="I89" t="n">
         <v>1140000000</v>
       </c>
+      <c r="J89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2898,6 +2991,7 @@
       <c r="I90" t="n">
         <v>1140000000</v>
       </c>
+      <c r="J90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2927,6 +3021,7 @@
       <c r="I91" t="n">
         <v>1140000000</v>
       </c>
+      <c r="J91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2956,6 +3051,7 @@
       <c r="I92" t="n">
         <v>1140000000</v>
       </c>
+      <c r="J92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2975,6 +3071,7 @@
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3002,6 +3099,7 @@
       <c r="I94" t="n">
         <v>1400000000</v>
       </c>
+      <c r="J94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3029,6 +3127,7 @@
       <c r="I95" t="n">
         <v>1400000000</v>
       </c>
+      <c r="J95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3056,6 +3155,7 @@
       <c r="I96" t="n">
         <v>1400000000</v>
       </c>
+      <c r="J96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3085,6 +3185,7 @@
       <c r="I97" t="n">
         <v>1400000000</v>
       </c>
+      <c r="J97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3114,6 +3215,7 @@
       <c r="I98" t="n">
         <v>1400000000</v>
       </c>
+      <c r="J98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3133,6 +3235,7 @@
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr"/>
       <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3160,6 +3263,7 @@
       <c r="I100" t="n">
         <v>4861655658</v>
       </c>
+      <c r="J100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3187,6 +3291,7 @@
       <c r="I101" t="n">
         <v>4861655783</v>
       </c>
+      <c r="J101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3214,6 +3319,7 @@
       <c r="I102" t="n">
         <v>4861655783</v>
       </c>
+      <c r="J102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3245,6 +3351,7 @@
       <c r="I103" t="n">
         <v>4861655783</v>
       </c>
+      <c r="J103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3276,6 +3383,7 @@
       <c r="I104" t="n">
         <v>4861655783</v>
       </c>
+      <c r="J104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3295,6 +3403,7 @@
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3322,6 +3431,7 @@
       <c r="I106" t="n">
         <v>2534400000</v>
       </c>
+      <c r="J106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3349,6 +3459,7 @@
       <c r="I107" t="n">
         <v>2534400000</v>
       </c>
+      <c r="J107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3376,6 +3487,7 @@
       <c r="I108" t="n">
         <v>2534400000</v>
       </c>
+      <c r="J108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3405,6 +3517,7 @@
       <c r="I109" t="n">
         <v>2534400000</v>
       </c>
+      <c r="J109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3434,6 +3547,7 @@
       <c r="I110" t="n">
         <v>2534400000</v>
       </c>
+      <c r="J110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3453,6 +3567,7 @@
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="inlineStr"/>
       <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3480,6 +3595,7 @@
       <c r="I112" t="n">
         <v>500000000</v>
       </c>
+      <c r="J112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -3507,6 +3623,7 @@
       <c r="I113" t="n">
         <v>500000000</v>
       </c>
+      <c r="J113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -3534,6 +3651,7 @@
       <c r="I114" t="n">
         <v>500000000</v>
       </c>
+      <c r="J114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -3565,6 +3683,7 @@
       <c r="I115" t="n">
         <v>500000000</v>
       </c>
+      <c r="J115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -3596,6 +3715,7 @@
       <c r="I116" t="n">
         <v>500000000</v>
       </c>
+      <c r="J116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3615,6 +3735,7 @@
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr"/>
       <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3642,6 +3763,7 @@
       <c r="I118" t="n">
         <v>2100375969</v>
       </c>
+      <c r="J118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3669,6 +3791,7 @@
       <c r="I119" t="n">
         <v>2100375969</v>
       </c>
+      <c r="J119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3696,6 +3819,7 @@
       <c r="I120" t="n">
         <v>2100375969</v>
       </c>
+      <c r="J120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3725,6 +3849,7 @@
       <c r="I121" t="n">
         <v>2100375969</v>
       </c>
+      <c r="J121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3754,6 +3879,7 @@
       <c r="I122" t="n">
         <v>2100375969</v>
       </c>
+      <c r="J122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3781,6 +3907,7 @@
       <c r="I123" t="n">
         <v>43280112944</v>
       </c>
+      <c r="J123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3808,6 +3935,7 @@
       <c r="I124" t="n">
         <v>43280112945</v>
       </c>
+      <c r="J124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3835,6 +3963,7 @@
       <c r="I125" t="n">
         <v>43815615361</v>
       </c>
+      <c r="J125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3866,6 +3995,7 @@
       <c r="I126" t="n">
         <v>43815615361</v>
       </c>
+      <c r="J126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -3895,6 +4025,7 @@
       <c r="I127" t="n">
         <v>43815615361</v>
       </c>
+      <c r="J127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3914,6 +4045,7 @@
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="inlineStr"/>
       <c r="I128" t="inlineStr"/>
+      <c r="J128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3941,6 +4073,7 @@
       <c r="I129" t="n">
         <v>3063214056</v>
       </c>
+      <c r="J129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3968,6 +4101,7 @@
       <c r="I130" t="n">
         <v>3063214056</v>
       </c>
+      <c r="J130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3995,6 +4129,7 @@
       <c r="I131" t="n">
         <v>3063214056</v>
       </c>
+      <c r="J131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -4026,6 +4161,7 @@
       <c r="I132" t="n">
         <v>3063214056</v>
       </c>
+      <c r="J132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -4057,6 +4193,7 @@
       <c r="I133" t="n">
         <v>3063214056</v>
       </c>
+      <c r="J133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -4084,6 +4221,7 @@
       <c r="I134" t="n">
         <v>363281250</v>
       </c>
+      <c r="J134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -4111,6 +4249,7 @@
       <c r="I135" t="n">
         <v>363281250</v>
       </c>
+      <c r="J135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -4138,6 +4277,7 @@
       <c r="I136" t="n">
         <v>363281250</v>
       </c>
+      <c r="J136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4169,6 +4309,7 @@
       <c r="I137" t="n">
         <v>363281250</v>
       </c>
+      <c r="J137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -4200,6 +4341,7 @@
       <c r="I138" t="n">
         <v>363281250</v>
       </c>
+      <c r="J138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -4219,6 +4361,7 @@
       <c r="G139" t="inlineStr"/>
       <c r="H139" t="inlineStr"/>
       <c r="I139" t="inlineStr"/>
+      <c r="J139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -4246,6 +4389,7 @@
       <c r="I140" t="n">
         <v>2179104795</v>
       </c>
+      <c r="J140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -4273,6 +4417,7 @@
       <c r="I141" t="n">
         <v>2200000000</v>
       </c>
+      <c r="J141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -4300,6 +4445,7 @@
       <c r="I142" t="n">
         <v>2200000000</v>
       </c>
+      <c r="J142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -4331,6 +4477,7 @@
       <c r="I143" t="n">
         <v>2178536499</v>
       </c>
+      <c r="J143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -4362,6 +4509,7 @@
       <c r="I144" t="n">
         <v>2178536499</v>
       </c>
+      <c r="J144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -4381,6 +4529,7 @@
       <c r="G145" t="inlineStr"/>
       <c r="H145" t="inlineStr"/>
       <c r="I145" t="inlineStr"/>
+      <c r="J145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -4408,6 +4557,7 @@
       <c r="I146" t="n">
         <v>1375202955</v>
       </c>
+      <c r="J146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -4435,6 +4585,7 @@
       <c r="I147" t="n">
         <v>1379944589</v>
       </c>
+      <c r="J147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -4462,6 +4613,7 @@
       <c r="I148" t="n">
         <v>1379944589</v>
       </c>
+      <c r="J148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -4493,6 +4645,7 @@
       <c r="I149" t="n">
         <v>1379937237</v>
       </c>
+      <c r="J149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -4524,6 +4677,7 @@
       <c r="I150" t="n">
         <v>1373660993</v>
       </c>
+      <c r="J150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -4551,6 +4705,7 @@
       <c r="I151" t="n">
         <v>500000000</v>
       </c>
+      <c r="J151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -4578,6 +4733,7 @@
       <c r="I152" t="n">
         <v>500000000</v>
       </c>
+      <c r="J152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -4605,6 +4761,7 @@
       <c r="I153" t="n">
         <v>500000000</v>
       </c>
+      <c r="J153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -4636,6 +4793,7 @@
       <c r="I154" t="n">
         <v>500000000</v>
       </c>
+      <c r="J154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -4663,6 +4821,7 @@
       <c r="I155" t="n">
         <v>2800000000</v>
       </c>
+      <c r="J155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -4690,6 +4849,7 @@
       <c r="I156" t="n">
         <v>2800000000</v>
       </c>
+      <c r="J156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -4717,6 +4877,7 @@
       <c r="I157" t="n">
         <v>2800000000</v>
       </c>
+      <c r="J157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -4748,6 +4909,7 @@
       <c r="I158" t="n">
         <v>2800000000</v>
       </c>
+      <c r="J158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -4779,6 +4941,7 @@
       <c r="I159" t="n">
         <v>2800000000</v>
       </c>
+      <c r="J159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -4806,6 +4969,7 @@
       <c r="I160" t="n">
         <v>3500000000</v>
       </c>
+      <c r="J160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -4833,6 +4997,7 @@
       <c r="I161" t="n">
         <v>3500000000</v>
       </c>
+      <c r="J161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -4860,6 +5025,7 @@
       <c r="I162" t="n">
         <v>3500000000</v>
       </c>
+      <c r="J162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -4891,6 +5057,7 @@
       <c r="I163" t="n">
         <v>3500000000</v>
       </c>
+      <c r="J163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -4922,6 +5089,7 @@
       <c r="I164" t="n">
         <v>3500000000</v>
       </c>
+      <c r="J164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -4941,6 +5109,7 @@
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="inlineStr"/>
       <c r="I165" t="inlineStr"/>
+      <c r="J165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -4968,6 +5137,7 @@
       <c r="I166" t="n">
         <v>1926795598</v>
       </c>
+      <c r="J166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -4995,6 +5165,7 @@
       <c r="I167" t="n">
         <v>1926795598</v>
       </c>
+      <c r="J167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -5022,6 +5193,7 @@
       <c r="I168" t="n">
         <v>1926795598</v>
       </c>
+      <c r="J168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -5053,6 +5225,7 @@
       <c r="I169" t="n">
         <v>1926795598</v>
       </c>
+      <c r="J169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -5084,6 +5257,7 @@
       <c r="I170" t="n">
         <v>1926795598</v>
       </c>
+      <c r="J170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -5111,6 +5285,7 @@
       <c r="I171" t="n">
         <v>8447051000</v>
       </c>
+      <c r="J171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -5138,6 +5313,7 @@
       <c r="I172" t="n">
         <v>8447051000</v>
       </c>
+      <c r="J172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -5165,6 +5341,7 @@
       <c r="I173" t="n">
         <v>8447051000</v>
       </c>
+      <c r="J173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -5196,6 +5373,7 @@
       <c r="I174" t="n">
         <v>8447051000</v>
       </c>
+      <c r="J174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -5226,6 +5404,3373 @@
       </c>
       <c r="I175" t="n">
         <v>8447051000</v>
+      </c>
+      <c r="J175" t="inlineStr"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>MGROS.IS</t>
+        </is>
+      </c>
+      <c r="B176" s="1" t="n">
+        <v>43921</v>
+      </c>
+      <c r="C176" t="n">
+        <v>0</v>
+      </c>
+      <c r="D176" t="n">
+        <v>0</v>
+      </c>
+      <c r="E176" t="n">
+        <v>0</v>
+      </c>
+      <c r="F176" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G176" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H176" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I176" t="n">
+        <v>0</v>
+      </c>
+      <c r="J176" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>MGROS.IS</t>
+        </is>
+      </c>
+      <c r="B177" s="1" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C177" t="n">
+        <v>0</v>
+      </c>
+      <c r="D177" t="n">
+        <v>0</v>
+      </c>
+      <c r="E177" t="n">
+        <v>0</v>
+      </c>
+      <c r="F177" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G177" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H177" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I177" t="n">
+        <v>0</v>
+      </c>
+      <c r="J177" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>MGROS.IS</t>
+        </is>
+      </c>
+      <c r="B178" s="1" t="n">
+        <v>44286</v>
+      </c>
+      <c r="C178" t="n">
+        <v>0</v>
+      </c>
+      <c r="D178" t="n">
+        <v>0</v>
+      </c>
+      <c r="E178" t="n">
+        <v>0</v>
+      </c>
+      <c r="F178" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G178" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H178" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I178" t="n">
+        <v>0</v>
+      </c>
+      <c r="J178" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>MGROS.IS</t>
+        </is>
+      </c>
+      <c r="B179" s="1" t="n">
+        <v>44469</v>
+      </c>
+      <c r="C179" t="n">
+        <v>0</v>
+      </c>
+      <c r="D179" t="n">
+        <v>0</v>
+      </c>
+      <c r="E179" t="n">
+        <v>0</v>
+      </c>
+      <c r="F179" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G179" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H179" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I179" t="n">
+        <v>0</v>
+      </c>
+      <c r="J179" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>MGROS.IS</t>
+        </is>
+      </c>
+      <c r="B180" s="1" t="n">
+        <v>44651</v>
+      </c>
+      <c r="C180" t="n">
+        <v>0</v>
+      </c>
+      <c r="D180" t="n">
+        <v>0</v>
+      </c>
+      <c r="E180" t="n">
+        <v>0</v>
+      </c>
+      <c r="F180" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G180" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H180" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I180" t="n">
+        <v>0</v>
+      </c>
+      <c r="J180" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>MGROS.IS</t>
+        </is>
+      </c>
+      <c r="B181" s="1" t="n">
+        <v>44834</v>
+      </c>
+      <c r="C181" t="n">
+        <v>0</v>
+      </c>
+      <c r="D181" t="n">
+        <v>0</v>
+      </c>
+      <c r="E181" t="n">
+        <v>0</v>
+      </c>
+      <c r="F181" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G181" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H181" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I181" t="n">
+        <v>0</v>
+      </c>
+      <c r="J181" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>MGROS.IS</t>
+        </is>
+      </c>
+      <c r="B182" s="1" t="n">
+        <v>45016</v>
+      </c>
+      <c r="C182" t="n">
+        <v>0</v>
+      </c>
+      <c r="D182" t="n">
+        <v>0</v>
+      </c>
+      <c r="E182" t="n">
+        <v>0</v>
+      </c>
+      <c r="F182" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G182" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H182" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I182" t="n">
+        <v>0</v>
+      </c>
+      <c r="J182" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>MGROS.IS</t>
+        </is>
+      </c>
+      <c r="B183" s="1" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C183" t="n">
+        <v>0</v>
+      </c>
+      <c r="D183" t="n">
+        <v>0</v>
+      </c>
+      <c r="E183" t="n">
+        <v>0</v>
+      </c>
+      <c r="F183" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G183" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H183" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I183" t="n">
+        <v>0</v>
+      </c>
+      <c r="J183" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>MGROS.IS</t>
+        </is>
+      </c>
+      <c r="B184" s="1" t="n">
+        <v>45382</v>
+      </c>
+      <c r="C184" t="n">
+        <v>0</v>
+      </c>
+      <c r="D184" t="n">
+        <v>0</v>
+      </c>
+      <c r="E184" t="n">
+        <v>0</v>
+      </c>
+      <c r="F184" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G184" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H184" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I184" t="n">
+        <v>0</v>
+      </c>
+      <c r="J184" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>MGROS.IS</t>
+        </is>
+      </c>
+      <c r="B185" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="C185" t="n">
+        <v>0</v>
+      </c>
+      <c r="D185" t="n">
+        <v>0</v>
+      </c>
+      <c r="E185" t="n">
+        <v>0</v>
+      </c>
+      <c r="F185" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G185" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H185" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I185" t="n">
+        <v>0</v>
+      </c>
+      <c r="J185" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>MGROS.IS</t>
+        </is>
+      </c>
+      <c r="B186" s="1" t="n">
+        <v>45747</v>
+      </c>
+      <c r="C186" t="n">
+        <v>0</v>
+      </c>
+      <c r="D186" t="n">
+        <v>0</v>
+      </c>
+      <c r="E186" t="n">
+        <v>0</v>
+      </c>
+      <c r="F186" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G186" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H186" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I186" t="n">
+        <v>0</v>
+      </c>
+      <c r="J186" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>TTRAK.IS</t>
+        </is>
+      </c>
+      <c r="B187" s="1" t="n">
+        <v>43921</v>
+      </c>
+      <c r="C187" t="n">
+        <v>0</v>
+      </c>
+      <c r="D187" t="n">
+        <v>0</v>
+      </c>
+      <c r="E187" t="n">
+        <v>0</v>
+      </c>
+      <c r="F187" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G187" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H187" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I187" t="n">
+        <v>0</v>
+      </c>
+      <c r="J187" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>TTRAK.IS</t>
+        </is>
+      </c>
+      <c r="B188" s="1" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C188" t="n">
+        <v>0</v>
+      </c>
+      <c r="D188" t="n">
+        <v>0</v>
+      </c>
+      <c r="E188" t="n">
+        <v>0</v>
+      </c>
+      <c r="F188" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G188" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H188" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I188" t="n">
+        <v>0</v>
+      </c>
+      <c r="J188" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>TTRAK.IS</t>
+        </is>
+      </c>
+      <c r="B189" s="1" t="n">
+        <v>44286</v>
+      </c>
+      <c r="C189" t="n">
+        <v>0</v>
+      </c>
+      <c r="D189" t="n">
+        <v>0</v>
+      </c>
+      <c r="E189" t="n">
+        <v>0</v>
+      </c>
+      <c r="F189" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G189" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H189" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I189" t="n">
+        <v>0</v>
+      </c>
+      <c r="J189" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>TTRAK.IS</t>
+        </is>
+      </c>
+      <c r="B190" s="1" t="n">
+        <v>44469</v>
+      </c>
+      <c r="C190" t="n">
+        <v>0</v>
+      </c>
+      <c r="D190" t="n">
+        <v>0</v>
+      </c>
+      <c r="E190" t="n">
+        <v>0</v>
+      </c>
+      <c r="F190" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G190" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H190" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I190" t="n">
+        <v>0</v>
+      </c>
+      <c r="J190" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>TTRAK.IS</t>
+        </is>
+      </c>
+      <c r="B191" s="1" t="n">
+        <v>44651</v>
+      </c>
+      <c r="C191" t="n">
+        <v>0</v>
+      </c>
+      <c r="D191" t="n">
+        <v>0</v>
+      </c>
+      <c r="E191" t="n">
+        <v>0</v>
+      </c>
+      <c r="F191" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G191" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H191" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I191" t="n">
+        <v>0</v>
+      </c>
+      <c r="J191" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>TTRAK.IS</t>
+        </is>
+      </c>
+      <c r="B192" s="1" t="n">
+        <v>44834</v>
+      </c>
+      <c r="C192" t="n">
+        <v>0</v>
+      </c>
+      <c r="D192" t="n">
+        <v>0</v>
+      </c>
+      <c r="E192" t="n">
+        <v>0</v>
+      </c>
+      <c r="F192" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G192" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H192" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I192" t="n">
+        <v>0</v>
+      </c>
+      <c r="J192" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>TTRAK.IS</t>
+        </is>
+      </c>
+      <c r="B193" s="1" t="n">
+        <v>45016</v>
+      </c>
+      <c r="C193" t="n">
+        <v>0</v>
+      </c>
+      <c r="D193" t="n">
+        <v>0</v>
+      </c>
+      <c r="E193" t="n">
+        <v>0</v>
+      </c>
+      <c r="F193" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G193" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H193" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I193" t="n">
+        <v>0</v>
+      </c>
+      <c r="J193" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>TTRAK.IS</t>
+        </is>
+      </c>
+      <c r="B194" s="1" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C194" t="n">
+        <v>0</v>
+      </c>
+      <c r="D194" t="n">
+        <v>0</v>
+      </c>
+      <c r="E194" t="n">
+        <v>0</v>
+      </c>
+      <c r="F194" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G194" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H194" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I194" t="n">
+        <v>0</v>
+      </c>
+      <c r="J194" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>TTRAK.IS</t>
+        </is>
+      </c>
+      <c r="B195" s="1" t="n">
+        <v>45382</v>
+      </c>
+      <c r="C195" t="n">
+        <v>0</v>
+      </c>
+      <c r="D195" t="n">
+        <v>0</v>
+      </c>
+      <c r="E195" t="n">
+        <v>0</v>
+      </c>
+      <c r="F195" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G195" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H195" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I195" t="n">
+        <v>0</v>
+      </c>
+      <c r="J195" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>TTRAK.IS</t>
+        </is>
+      </c>
+      <c r="B196" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="C196" t="n">
+        <v>0</v>
+      </c>
+      <c r="D196" t="n">
+        <v>0</v>
+      </c>
+      <c r="E196" t="n">
+        <v>0</v>
+      </c>
+      <c r="F196" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G196" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H196" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I196" t="n">
+        <v>0</v>
+      </c>
+      <c r="J196" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>TTRAK.IS</t>
+        </is>
+      </c>
+      <c r="B197" s="1" t="n">
+        <v>45747</v>
+      </c>
+      <c r="C197" t="n">
+        <v>0</v>
+      </c>
+      <c r="D197" t="n">
+        <v>0</v>
+      </c>
+      <c r="E197" t="n">
+        <v>0</v>
+      </c>
+      <c r="F197" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G197" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H197" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I197" t="n">
+        <v>0</v>
+      </c>
+      <c r="J197" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>HALKB.IS</t>
+        </is>
+      </c>
+      <c r="B198" s="1" t="n">
+        <v>43921</v>
+      </c>
+      <c r="C198" t="n">
+        <v>0</v>
+      </c>
+      <c r="D198" t="n">
+        <v>0</v>
+      </c>
+      <c r="E198" t="n">
+        <v>0</v>
+      </c>
+      <c r="F198" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G198" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H198" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I198" t="n">
+        <v>0</v>
+      </c>
+      <c r="J198" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>HALKB.IS</t>
+        </is>
+      </c>
+      <c r="B199" s="1" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C199" t="n">
+        <v>0</v>
+      </c>
+      <c r="D199" t="n">
+        <v>0</v>
+      </c>
+      <c r="E199" t="n">
+        <v>0</v>
+      </c>
+      <c r="F199" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G199" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H199" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I199" t="n">
+        <v>0</v>
+      </c>
+      <c r="J199" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>HALKB.IS</t>
+        </is>
+      </c>
+      <c r="B200" s="1" t="n">
+        <v>44286</v>
+      </c>
+      <c r="C200" t="n">
+        <v>0</v>
+      </c>
+      <c r="D200" t="n">
+        <v>0</v>
+      </c>
+      <c r="E200" t="n">
+        <v>0</v>
+      </c>
+      <c r="F200" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G200" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H200" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I200" t="n">
+        <v>0</v>
+      </c>
+      <c r="J200" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>HALKB.IS</t>
+        </is>
+      </c>
+      <c r="B201" s="1" t="n">
+        <v>44469</v>
+      </c>
+      <c r="C201" t="n">
+        <v>0</v>
+      </c>
+      <c r="D201" t="n">
+        <v>0</v>
+      </c>
+      <c r="E201" t="n">
+        <v>0</v>
+      </c>
+      <c r="F201" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G201" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H201" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I201" t="n">
+        <v>0</v>
+      </c>
+      <c r="J201" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>HALKB.IS</t>
+        </is>
+      </c>
+      <c r="B202" s="1" t="n">
+        <v>44651</v>
+      </c>
+      <c r="C202" t="n">
+        <v>0</v>
+      </c>
+      <c r="D202" t="n">
+        <v>0</v>
+      </c>
+      <c r="E202" t="n">
+        <v>0</v>
+      </c>
+      <c r="F202" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G202" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H202" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I202" t="n">
+        <v>0</v>
+      </c>
+      <c r="J202" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>HALKB.IS</t>
+        </is>
+      </c>
+      <c r="B203" s="1" t="n">
+        <v>44834</v>
+      </c>
+      <c r="C203" t="n">
+        <v>0</v>
+      </c>
+      <c r="D203" t="n">
+        <v>0</v>
+      </c>
+      <c r="E203" t="n">
+        <v>0</v>
+      </c>
+      <c r="F203" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G203" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H203" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I203" t="n">
+        <v>0</v>
+      </c>
+      <c r="J203" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>HALKB.IS</t>
+        </is>
+      </c>
+      <c r="B204" s="1" t="n">
+        <v>45016</v>
+      </c>
+      <c r="C204" t="n">
+        <v>0</v>
+      </c>
+      <c r="D204" t="n">
+        <v>0</v>
+      </c>
+      <c r="E204" t="n">
+        <v>0</v>
+      </c>
+      <c r="F204" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G204" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H204" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I204" t="n">
+        <v>0</v>
+      </c>
+      <c r="J204" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>HALKB.IS</t>
+        </is>
+      </c>
+      <c r="B205" s="1" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C205" t="n">
+        <v>0</v>
+      </c>
+      <c r="D205" t="n">
+        <v>0</v>
+      </c>
+      <c r="E205" t="n">
+        <v>0</v>
+      </c>
+      <c r="F205" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G205" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H205" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I205" t="n">
+        <v>0</v>
+      </c>
+      <c r="J205" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>HALKB.IS</t>
+        </is>
+      </c>
+      <c r="B206" s="1" t="n">
+        <v>45382</v>
+      </c>
+      <c r="C206" t="n">
+        <v>0</v>
+      </c>
+      <c r="D206" t="n">
+        <v>0</v>
+      </c>
+      <c r="E206" t="n">
+        <v>0</v>
+      </c>
+      <c r="F206" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G206" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H206" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I206" t="n">
+        <v>0</v>
+      </c>
+      <c r="J206" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>HALKB.IS</t>
+        </is>
+      </c>
+      <c r="B207" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="C207" t="n">
+        <v>0</v>
+      </c>
+      <c r="D207" t="n">
+        <v>0</v>
+      </c>
+      <c r="E207" t="n">
+        <v>0</v>
+      </c>
+      <c r="F207" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G207" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H207" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I207" t="n">
+        <v>0</v>
+      </c>
+      <c r="J207" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>HALKB.IS</t>
+        </is>
+      </c>
+      <c r="B208" s="1" t="n">
+        <v>45747</v>
+      </c>
+      <c r="C208" t="n">
+        <v>0</v>
+      </c>
+      <c r="D208" t="n">
+        <v>0</v>
+      </c>
+      <c r="E208" t="n">
+        <v>0</v>
+      </c>
+      <c r="F208" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G208" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H208" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I208" t="n">
+        <v>0</v>
+      </c>
+      <c r="J208" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>AGHOL.IS</t>
+        </is>
+      </c>
+      <c r="B209" s="1" t="n">
+        <v>43921</v>
+      </c>
+      <c r="C209" t="n">
+        <v>0</v>
+      </c>
+      <c r="D209" t="n">
+        <v>0</v>
+      </c>
+      <c r="E209" t="n">
+        <v>0</v>
+      </c>
+      <c r="F209" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G209" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H209" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I209" t="n">
+        <v>0</v>
+      </c>
+      <c r="J209" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>AGHOL.IS</t>
+        </is>
+      </c>
+      <c r="B210" s="1" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C210" t="n">
+        <v>0</v>
+      </c>
+      <c r="D210" t="n">
+        <v>0</v>
+      </c>
+      <c r="E210" t="n">
+        <v>0</v>
+      </c>
+      <c r="F210" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G210" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H210" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I210" t="n">
+        <v>0</v>
+      </c>
+      <c r="J210" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>AGHOL.IS</t>
+        </is>
+      </c>
+      <c r="B211" s="1" t="n">
+        <v>44286</v>
+      </c>
+      <c r="C211" t="n">
+        <v>0</v>
+      </c>
+      <c r="D211" t="n">
+        <v>0</v>
+      </c>
+      <c r="E211" t="n">
+        <v>0</v>
+      </c>
+      <c r="F211" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G211" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H211" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I211" t="n">
+        <v>0</v>
+      </c>
+      <c r="J211" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>AGHOL.IS</t>
+        </is>
+      </c>
+      <c r="B212" s="1" t="n">
+        <v>44469</v>
+      </c>
+      <c r="C212" t="n">
+        <v>0</v>
+      </c>
+      <c r="D212" t="n">
+        <v>0</v>
+      </c>
+      <c r="E212" t="n">
+        <v>0</v>
+      </c>
+      <c r="F212" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G212" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H212" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I212" t="n">
+        <v>0</v>
+      </c>
+      <c r="J212" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>AGHOL.IS</t>
+        </is>
+      </c>
+      <c r="B213" s="1" t="n">
+        <v>44651</v>
+      </c>
+      <c r="C213" t="n">
+        <v>0</v>
+      </c>
+      <c r="D213" t="n">
+        <v>0</v>
+      </c>
+      <c r="E213" t="n">
+        <v>0</v>
+      </c>
+      <c r="F213" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G213" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H213" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I213" t="n">
+        <v>0</v>
+      </c>
+      <c r="J213" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>AGHOL.IS</t>
+        </is>
+      </c>
+      <c r="B214" s="1" t="n">
+        <v>44834</v>
+      </c>
+      <c r="C214" t="n">
+        <v>0</v>
+      </c>
+      <c r="D214" t="n">
+        <v>0</v>
+      </c>
+      <c r="E214" t="n">
+        <v>0</v>
+      </c>
+      <c r="F214" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G214" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H214" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I214" t="n">
+        <v>0</v>
+      </c>
+      <c r="J214" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>AGHOL.IS</t>
+        </is>
+      </c>
+      <c r="B215" s="1" t="n">
+        <v>45016</v>
+      </c>
+      <c r="C215" t="n">
+        <v>0</v>
+      </c>
+      <c r="D215" t="n">
+        <v>0</v>
+      </c>
+      <c r="E215" t="n">
+        <v>0</v>
+      </c>
+      <c r="F215" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G215" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H215" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I215" t="n">
+        <v>0</v>
+      </c>
+      <c r="J215" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>AGHOL.IS</t>
+        </is>
+      </c>
+      <c r="B216" s="1" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C216" t="n">
+        <v>0</v>
+      </c>
+      <c r="D216" t="n">
+        <v>0</v>
+      </c>
+      <c r="E216" t="n">
+        <v>0</v>
+      </c>
+      <c r="F216" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G216" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H216" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I216" t="n">
+        <v>0</v>
+      </c>
+      <c r="J216" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>AGHOL.IS</t>
+        </is>
+      </c>
+      <c r="B217" s="1" t="n">
+        <v>45382</v>
+      </c>
+      <c r="C217" t="n">
+        <v>0</v>
+      </c>
+      <c r="D217" t="n">
+        <v>0</v>
+      </c>
+      <c r="E217" t="n">
+        <v>0</v>
+      </c>
+      <c r="F217" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G217" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H217" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I217" t="n">
+        <v>0</v>
+      </c>
+      <c r="J217" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>AGHOL.IS</t>
+        </is>
+      </c>
+      <c r="B218" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="C218" t="n">
+        <v>0</v>
+      </c>
+      <c r="D218" t="n">
+        <v>0</v>
+      </c>
+      <c r="E218" t="n">
+        <v>0</v>
+      </c>
+      <c r="F218" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G218" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H218" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I218" t="n">
+        <v>0</v>
+      </c>
+      <c r="J218" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>AGHOL.IS</t>
+        </is>
+      </c>
+      <c r="B219" s="1" t="n">
+        <v>45747</v>
+      </c>
+      <c r="C219" t="n">
+        <v>0</v>
+      </c>
+      <c r="D219" t="n">
+        <v>0</v>
+      </c>
+      <c r="E219" t="n">
+        <v>0</v>
+      </c>
+      <c r="F219" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G219" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H219" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I219" t="n">
+        <v>0</v>
+      </c>
+      <c r="J219" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>OTKAR.IS</t>
+        </is>
+      </c>
+      <c r="B220" s="1" t="n">
+        <v>43921</v>
+      </c>
+      <c r="C220" t="n">
+        <v>0</v>
+      </c>
+      <c r="D220" t="n">
+        <v>0</v>
+      </c>
+      <c r="E220" t="n">
+        <v>0</v>
+      </c>
+      <c r="F220" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G220" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H220" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I220" t="n">
+        <v>0</v>
+      </c>
+      <c r="J220" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>OTKAR.IS</t>
+        </is>
+      </c>
+      <c r="B221" s="1" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C221" t="n">
+        <v>0</v>
+      </c>
+      <c r="D221" t="n">
+        <v>0</v>
+      </c>
+      <c r="E221" t="n">
+        <v>0</v>
+      </c>
+      <c r="F221" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G221" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H221" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I221" t="n">
+        <v>0</v>
+      </c>
+      <c r="J221" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>OTKAR.IS</t>
+        </is>
+      </c>
+      <c r="B222" s="1" t="n">
+        <v>44286</v>
+      </c>
+      <c r="C222" t="n">
+        <v>0</v>
+      </c>
+      <c r="D222" t="n">
+        <v>0</v>
+      </c>
+      <c r="E222" t="n">
+        <v>0</v>
+      </c>
+      <c r="F222" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G222" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H222" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I222" t="n">
+        <v>0</v>
+      </c>
+      <c r="J222" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>OTKAR.IS</t>
+        </is>
+      </c>
+      <c r="B223" s="1" t="n">
+        <v>44469</v>
+      </c>
+      <c r="C223" t="n">
+        <v>0</v>
+      </c>
+      <c r="D223" t="n">
+        <v>0</v>
+      </c>
+      <c r="E223" t="n">
+        <v>0</v>
+      </c>
+      <c r="F223" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G223" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H223" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I223" t="n">
+        <v>0</v>
+      </c>
+      <c r="J223" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>OTKAR.IS</t>
+        </is>
+      </c>
+      <c r="B224" s="1" t="n">
+        <v>44651</v>
+      </c>
+      <c r="C224" t="n">
+        <v>0</v>
+      </c>
+      <c r="D224" t="n">
+        <v>0</v>
+      </c>
+      <c r="E224" t="n">
+        <v>0</v>
+      </c>
+      <c r="F224" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G224" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H224" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I224" t="n">
+        <v>0</v>
+      </c>
+      <c r="J224" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>OTKAR.IS</t>
+        </is>
+      </c>
+      <c r="B225" s="1" t="n">
+        <v>44834</v>
+      </c>
+      <c r="C225" t="n">
+        <v>0</v>
+      </c>
+      <c r="D225" t="n">
+        <v>0</v>
+      </c>
+      <c r="E225" t="n">
+        <v>0</v>
+      </c>
+      <c r="F225" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G225" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H225" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I225" t="n">
+        <v>0</v>
+      </c>
+      <c r="J225" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>OTKAR.IS</t>
+        </is>
+      </c>
+      <c r="B226" s="1" t="n">
+        <v>45016</v>
+      </c>
+      <c r="C226" t="n">
+        <v>0</v>
+      </c>
+      <c r="D226" t="n">
+        <v>0</v>
+      </c>
+      <c r="E226" t="n">
+        <v>0</v>
+      </c>
+      <c r="F226" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G226" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H226" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I226" t="n">
+        <v>0</v>
+      </c>
+      <c r="J226" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>OTKAR.IS</t>
+        </is>
+      </c>
+      <c r="B227" s="1" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C227" t="n">
+        <v>0</v>
+      </c>
+      <c r="D227" t="n">
+        <v>0</v>
+      </c>
+      <c r="E227" t="n">
+        <v>0</v>
+      </c>
+      <c r="F227" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G227" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H227" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I227" t="n">
+        <v>0</v>
+      </c>
+      <c r="J227" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>OTKAR.IS</t>
+        </is>
+      </c>
+      <c r="B228" s="1" t="n">
+        <v>45382</v>
+      </c>
+      <c r="C228" t="n">
+        <v>0</v>
+      </c>
+      <c r="D228" t="n">
+        <v>0</v>
+      </c>
+      <c r="E228" t="n">
+        <v>0</v>
+      </c>
+      <c r="F228" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G228" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H228" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I228" t="n">
+        <v>0</v>
+      </c>
+      <c r="J228" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>OTKAR.IS</t>
+        </is>
+      </c>
+      <c r="B229" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="C229" t="n">
+        <v>0</v>
+      </c>
+      <c r="D229" t="n">
+        <v>0</v>
+      </c>
+      <c r="E229" t="n">
+        <v>0</v>
+      </c>
+      <c r="F229" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G229" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H229" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I229" t="n">
+        <v>0</v>
+      </c>
+      <c r="J229" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>OTKAR.IS</t>
+        </is>
+      </c>
+      <c r="B230" s="1" t="n">
+        <v>45747</v>
+      </c>
+      <c r="C230" t="n">
+        <v>0</v>
+      </c>
+      <c r="D230" t="n">
+        <v>0</v>
+      </c>
+      <c r="E230" t="n">
+        <v>0</v>
+      </c>
+      <c r="F230" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G230" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H230" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I230" t="n">
+        <v>0</v>
+      </c>
+      <c r="J230" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>VAKBN.IS</t>
+        </is>
+      </c>
+      <c r="B231" s="1" t="n">
+        <v>43921</v>
+      </c>
+      <c r="C231" t="n">
+        <v>0</v>
+      </c>
+      <c r="D231" t="n">
+        <v>0</v>
+      </c>
+      <c r="E231" t="n">
+        <v>0</v>
+      </c>
+      <c r="F231" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G231" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H231" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I231" t="n">
+        <v>0</v>
+      </c>
+      <c r="J231" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>VAKBN.IS</t>
+        </is>
+      </c>
+      <c r="B232" s="1" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C232" t="n">
+        <v>0</v>
+      </c>
+      <c r="D232" t="n">
+        <v>0</v>
+      </c>
+      <c r="E232" t="n">
+        <v>0</v>
+      </c>
+      <c r="F232" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G232" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H232" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I232" t="n">
+        <v>0</v>
+      </c>
+      <c r="J232" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>VAKBN.IS</t>
+        </is>
+      </c>
+      <c r="B233" s="1" t="n">
+        <v>44286</v>
+      </c>
+      <c r="C233" t="n">
+        <v>0</v>
+      </c>
+      <c r="D233" t="n">
+        <v>0</v>
+      </c>
+      <c r="E233" t="n">
+        <v>0</v>
+      </c>
+      <c r="F233" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G233" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H233" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I233" t="n">
+        <v>0</v>
+      </c>
+      <c r="J233" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>VAKBN.IS</t>
+        </is>
+      </c>
+      <c r="B234" s="1" t="n">
+        <v>44469</v>
+      </c>
+      <c r="C234" t="n">
+        <v>0</v>
+      </c>
+      <c r="D234" t="n">
+        <v>0</v>
+      </c>
+      <c r="E234" t="n">
+        <v>0</v>
+      </c>
+      <c r="F234" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G234" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H234" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I234" t="n">
+        <v>0</v>
+      </c>
+      <c r="J234" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>VAKBN.IS</t>
+        </is>
+      </c>
+      <c r="B235" s="1" t="n">
+        <v>44651</v>
+      </c>
+      <c r="C235" t="n">
+        <v>0</v>
+      </c>
+      <c r="D235" t="n">
+        <v>0</v>
+      </c>
+      <c r="E235" t="n">
+        <v>0</v>
+      </c>
+      <c r="F235" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G235" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H235" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I235" t="n">
+        <v>0</v>
+      </c>
+      <c r="J235" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>VAKBN.IS</t>
+        </is>
+      </c>
+      <c r="B236" s="1" t="n">
+        <v>44834</v>
+      </c>
+      <c r="C236" t="n">
+        <v>0</v>
+      </c>
+      <c r="D236" t="n">
+        <v>0</v>
+      </c>
+      <c r="E236" t="n">
+        <v>0</v>
+      </c>
+      <c r="F236" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G236" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H236" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I236" t="n">
+        <v>0</v>
+      </c>
+      <c r="J236" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>VAKBN.IS</t>
+        </is>
+      </c>
+      <c r="B237" s="1" t="n">
+        <v>45016</v>
+      </c>
+      <c r="C237" t="n">
+        <v>0</v>
+      </c>
+      <c r="D237" t="n">
+        <v>0</v>
+      </c>
+      <c r="E237" t="n">
+        <v>0</v>
+      </c>
+      <c r="F237" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G237" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H237" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I237" t="n">
+        <v>0</v>
+      </c>
+      <c r="J237" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>VAKBN.IS</t>
+        </is>
+      </c>
+      <c r="B238" s="1" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C238" t="n">
+        <v>0</v>
+      </c>
+      <c r="D238" t="n">
+        <v>0</v>
+      </c>
+      <c r="E238" t="n">
+        <v>0</v>
+      </c>
+      <c r="F238" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G238" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H238" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I238" t="n">
+        <v>0</v>
+      </c>
+      <c r="J238" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>VAKBN.IS</t>
+        </is>
+      </c>
+      <c r="B239" s="1" t="n">
+        <v>45382</v>
+      </c>
+      <c r="C239" t="n">
+        <v>0</v>
+      </c>
+      <c r="D239" t="n">
+        <v>0</v>
+      </c>
+      <c r="E239" t="n">
+        <v>0</v>
+      </c>
+      <c r="F239" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G239" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H239" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I239" t="n">
+        <v>0</v>
+      </c>
+      <c r="J239" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>VAKBN.IS</t>
+        </is>
+      </c>
+      <c r="B240" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="C240" t="n">
+        <v>0</v>
+      </c>
+      <c r="D240" t="n">
+        <v>0</v>
+      </c>
+      <c r="E240" t="n">
+        <v>0</v>
+      </c>
+      <c r="F240" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G240" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H240" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I240" t="n">
+        <v>0</v>
+      </c>
+      <c r="J240" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>VAKBN.IS</t>
+        </is>
+      </c>
+      <c r="B241" s="1" t="n">
+        <v>45747</v>
+      </c>
+      <c r="C241" t="n">
+        <v>0</v>
+      </c>
+      <c r="D241" t="n">
+        <v>0</v>
+      </c>
+      <c r="E241" t="n">
+        <v>0</v>
+      </c>
+      <c r="F241" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G241" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H241" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I241" t="n">
+        <v>0</v>
+      </c>
+      <c r="J241" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>ALBRK.IS</t>
+        </is>
+      </c>
+      <c r="B242" s="1" t="n">
+        <v>43921</v>
+      </c>
+      <c r="C242" t="n">
+        <v>0</v>
+      </c>
+      <c r="D242" t="n">
+        <v>0</v>
+      </c>
+      <c r="E242" t="n">
+        <v>0</v>
+      </c>
+      <c r="F242" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G242" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H242" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I242" t="n">
+        <v>0</v>
+      </c>
+      <c r="J242" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>ALBRK.IS</t>
+        </is>
+      </c>
+      <c r="B243" s="1" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C243" t="n">
+        <v>0</v>
+      </c>
+      <c r="D243" t="n">
+        <v>0</v>
+      </c>
+      <c r="E243" t="n">
+        <v>0</v>
+      </c>
+      <c r="F243" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G243" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H243" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I243" t="n">
+        <v>0</v>
+      </c>
+      <c r="J243" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>ALBRK.IS</t>
+        </is>
+      </c>
+      <c r="B244" s="1" t="n">
+        <v>44286</v>
+      </c>
+      <c r="C244" t="n">
+        <v>0</v>
+      </c>
+      <c r="D244" t="n">
+        <v>0</v>
+      </c>
+      <c r="E244" t="n">
+        <v>0</v>
+      </c>
+      <c r="F244" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G244" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H244" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I244" t="n">
+        <v>0</v>
+      </c>
+      <c r="J244" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>ALBRK.IS</t>
+        </is>
+      </c>
+      <c r="B245" s="1" t="n">
+        <v>44469</v>
+      </c>
+      <c r="C245" t="n">
+        <v>0</v>
+      </c>
+      <c r="D245" t="n">
+        <v>0</v>
+      </c>
+      <c r="E245" t="n">
+        <v>0</v>
+      </c>
+      <c r="F245" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G245" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H245" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I245" t="n">
+        <v>0</v>
+      </c>
+      <c r="J245" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>ALBRK.IS</t>
+        </is>
+      </c>
+      <c r="B246" s="1" t="n">
+        <v>44651</v>
+      </c>
+      <c r="C246" t="n">
+        <v>0</v>
+      </c>
+      <c r="D246" t="n">
+        <v>0</v>
+      </c>
+      <c r="E246" t="n">
+        <v>0</v>
+      </c>
+      <c r="F246" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G246" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H246" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I246" t="n">
+        <v>0</v>
+      </c>
+      <c r="J246" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>ALBRK.IS</t>
+        </is>
+      </c>
+      <c r="B247" s="1" t="n">
+        <v>44834</v>
+      </c>
+      <c r="C247" t="n">
+        <v>0</v>
+      </c>
+      <c r="D247" t="n">
+        <v>0</v>
+      </c>
+      <c r="E247" t="n">
+        <v>0</v>
+      </c>
+      <c r="F247" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G247" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H247" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I247" t="n">
+        <v>0</v>
+      </c>
+      <c r="J247" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>ALBRK.IS</t>
+        </is>
+      </c>
+      <c r="B248" s="1" t="n">
+        <v>45016</v>
+      </c>
+      <c r="C248" t="n">
+        <v>0</v>
+      </c>
+      <c r="D248" t="n">
+        <v>0</v>
+      </c>
+      <c r="E248" t="n">
+        <v>0</v>
+      </c>
+      <c r="F248" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G248" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H248" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I248" t="n">
+        <v>0</v>
+      </c>
+      <c r="J248" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>ALBRK.IS</t>
+        </is>
+      </c>
+      <c r="B249" s="1" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C249" t="n">
+        <v>0</v>
+      </c>
+      <c r="D249" t="n">
+        <v>0</v>
+      </c>
+      <c r="E249" t="n">
+        <v>0</v>
+      </c>
+      <c r="F249" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G249" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H249" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I249" t="n">
+        <v>0</v>
+      </c>
+      <c r="J249" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>ALBRK.IS</t>
+        </is>
+      </c>
+      <c r="B250" s="1" t="n">
+        <v>45382</v>
+      </c>
+      <c r="C250" t="n">
+        <v>0</v>
+      </c>
+      <c r="D250" t="n">
+        <v>0</v>
+      </c>
+      <c r="E250" t="n">
+        <v>0</v>
+      </c>
+      <c r="F250" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G250" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H250" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I250" t="n">
+        <v>0</v>
+      </c>
+      <c r="J250" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>ALBRK.IS</t>
+        </is>
+      </c>
+      <c r="B251" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="C251" t="n">
+        <v>0</v>
+      </c>
+      <c r="D251" t="n">
+        <v>0</v>
+      </c>
+      <c r="E251" t="n">
+        <v>0</v>
+      </c>
+      <c r="F251" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G251" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H251" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I251" t="n">
+        <v>0</v>
+      </c>
+      <c r="J251" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>ALBRK.IS</t>
+        </is>
+      </c>
+      <c r="B252" s="1" t="n">
+        <v>45747</v>
+      </c>
+      <c r="C252" t="n">
+        <v>0</v>
+      </c>
+      <c r="D252" t="n">
+        <v>0</v>
+      </c>
+      <c r="E252" t="n">
+        <v>0</v>
+      </c>
+      <c r="F252" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G252" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H252" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I252" t="n">
+        <v>0</v>
+      </c>
+      <c r="J252" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>DOHOL.IS</t>
+        </is>
+      </c>
+      <c r="B253" s="1" t="n">
+        <v>43921</v>
+      </c>
+      <c r="C253" t="n">
+        <v>0</v>
+      </c>
+      <c r="D253" t="n">
+        <v>0</v>
+      </c>
+      <c r="E253" t="n">
+        <v>0</v>
+      </c>
+      <c r="F253" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G253" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H253" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I253" t="n">
+        <v>0</v>
+      </c>
+      <c r="J253" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>DOHOL.IS</t>
+        </is>
+      </c>
+      <c r="B254" s="1" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C254" t="n">
+        <v>0</v>
+      </c>
+      <c r="D254" t="n">
+        <v>0</v>
+      </c>
+      <c r="E254" t="n">
+        <v>0</v>
+      </c>
+      <c r="F254" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G254" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H254" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I254" t="n">
+        <v>0</v>
+      </c>
+      <c r="J254" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>DOHOL.IS</t>
+        </is>
+      </c>
+      <c r="B255" s="1" t="n">
+        <v>44286</v>
+      </c>
+      <c r="C255" t="n">
+        <v>0</v>
+      </c>
+      <c r="D255" t="n">
+        <v>0</v>
+      </c>
+      <c r="E255" t="n">
+        <v>0</v>
+      </c>
+      <c r="F255" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G255" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H255" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I255" t="n">
+        <v>0</v>
+      </c>
+      <c r="J255" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>DOHOL.IS</t>
+        </is>
+      </c>
+      <c r="B256" s="1" t="n">
+        <v>44469</v>
+      </c>
+      <c r="C256" t="n">
+        <v>0</v>
+      </c>
+      <c r="D256" t="n">
+        <v>0</v>
+      </c>
+      <c r="E256" t="n">
+        <v>0</v>
+      </c>
+      <c r="F256" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G256" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H256" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I256" t="n">
+        <v>0</v>
+      </c>
+      <c r="J256" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>DOHOL.IS</t>
+        </is>
+      </c>
+      <c r="B257" s="1" t="n">
+        <v>44651</v>
+      </c>
+      <c r="C257" t="n">
+        <v>0</v>
+      </c>
+      <c r="D257" t="n">
+        <v>0</v>
+      </c>
+      <c r="E257" t="n">
+        <v>0</v>
+      </c>
+      <c r="F257" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G257" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H257" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I257" t="n">
+        <v>0</v>
+      </c>
+      <c r="J257" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>DOHOL.IS</t>
+        </is>
+      </c>
+      <c r="B258" s="1" t="n">
+        <v>44834</v>
+      </c>
+      <c r="C258" t="n">
+        <v>0</v>
+      </c>
+      <c r="D258" t="n">
+        <v>0</v>
+      </c>
+      <c r="E258" t="n">
+        <v>0</v>
+      </c>
+      <c r="F258" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G258" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H258" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I258" t="n">
+        <v>0</v>
+      </c>
+      <c r="J258" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>DOHOL.IS</t>
+        </is>
+      </c>
+      <c r="B259" s="1" t="n">
+        <v>45016</v>
+      </c>
+      <c r="C259" t="n">
+        <v>0</v>
+      </c>
+      <c r="D259" t="n">
+        <v>0</v>
+      </c>
+      <c r="E259" t="n">
+        <v>0</v>
+      </c>
+      <c r="F259" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G259" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H259" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I259" t="n">
+        <v>0</v>
+      </c>
+      <c r="J259" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>DOHOL.IS</t>
+        </is>
+      </c>
+      <c r="B260" s="1" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C260" t="n">
+        <v>0</v>
+      </c>
+      <c r="D260" t="n">
+        <v>0</v>
+      </c>
+      <c r="E260" t="n">
+        <v>0</v>
+      </c>
+      <c r="F260" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G260" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H260" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I260" t="n">
+        <v>0</v>
+      </c>
+      <c r="J260" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>DOHOL.IS</t>
+        </is>
+      </c>
+      <c r="B261" s="1" t="n">
+        <v>45382</v>
+      </c>
+      <c r="C261" t="n">
+        <v>0</v>
+      </c>
+      <c r="D261" t="n">
+        <v>0</v>
+      </c>
+      <c r="E261" t="n">
+        <v>0</v>
+      </c>
+      <c r="F261" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G261" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H261" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I261" t="n">
+        <v>0</v>
+      </c>
+      <c r="J261" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>DOHOL.IS</t>
+        </is>
+      </c>
+      <c r="B262" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="C262" t="n">
+        <v>0</v>
+      </c>
+      <c r="D262" t="n">
+        <v>0</v>
+      </c>
+      <c r="E262" t="n">
+        <v>0</v>
+      </c>
+      <c r="F262" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G262" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H262" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I262" t="n">
+        <v>0</v>
+      </c>
+      <c r="J262" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>DOHOL.IS</t>
+        </is>
+      </c>
+      <c r="B263" s="1" t="n">
+        <v>45747</v>
+      </c>
+      <c r="C263" t="n">
+        <v>0</v>
+      </c>
+      <c r="D263" t="n">
+        <v>0</v>
+      </c>
+      <c r="E263" t="n">
+        <v>0</v>
+      </c>
+      <c r="F263" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G263" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H263" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I263" t="n">
+        <v>0</v>
+      </c>
+      <c r="J263" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>TEKFEN.IS</t>
+        </is>
+      </c>
+      <c r="B264" s="1" t="n">
+        <v>43921</v>
+      </c>
+      <c r="C264" t="n">
+        <v>0</v>
+      </c>
+      <c r="D264" t="n">
+        <v>0</v>
+      </c>
+      <c r="E264" t="n">
+        <v>0</v>
+      </c>
+      <c r="F264" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G264" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H264" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I264" t="n">
+        <v>0</v>
+      </c>
+      <c r="J264" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>TEKFEN.IS</t>
+        </is>
+      </c>
+      <c r="B265" s="1" t="n">
+        <v>44104</v>
+      </c>
+      <c r="C265" t="n">
+        <v>0</v>
+      </c>
+      <c r="D265" t="n">
+        <v>0</v>
+      </c>
+      <c r="E265" t="n">
+        <v>0</v>
+      </c>
+      <c r="F265" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G265" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H265" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I265" t="n">
+        <v>0</v>
+      </c>
+      <c r="J265" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>TEKFEN.IS</t>
+        </is>
+      </c>
+      <c r="B266" s="1" t="n">
+        <v>44286</v>
+      </c>
+      <c r="C266" t="n">
+        <v>0</v>
+      </c>
+      <c r="D266" t="n">
+        <v>0</v>
+      </c>
+      <c r="E266" t="n">
+        <v>0</v>
+      </c>
+      <c r="F266" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G266" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H266" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I266" t="n">
+        <v>0</v>
+      </c>
+      <c r="J266" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>TEKFEN.IS</t>
+        </is>
+      </c>
+      <c r="B267" s="1" t="n">
+        <v>44469</v>
+      </c>
+      <c r="C267" t="n">
+        <v>0</v>
+      </c>
+      <c r="D267" t="n">
+        <v>0</v>
+      </c>
+      <c r="E267" t="n">
+        <v>0</v>
+      </c>
+      <c r="F267" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G267" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H267" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I267" t="n">
+        <v>0</v>
+      </c>
+      <c r="J267" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>TEKFEN.IS</t>
+        </is>
+      </c>
+      <c r="B268" s="1" t="n">
+        <v>44651</v>
+      </c>
+      <c r="C268" t="n">
+        <v>0</v>
+      </c>
+      <c r="D268" t="n">
+        <v>0</v>
+      </c>
+      <c r="E268" t="n">
+        <v>0</v>
+      </c>
+      <c r="F268" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G268" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H268" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I268" t="n">
+        <v>0</v>
+      </c>
+      <c r="J268" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>TEKFEN.IS</t>
+        </is>
+      </c>
+      <c r="B269" s="1" t="n">
+        <v>44834</v>
+      </c>
+      <c r="C269" t="n">
+        <v>0</v>
+      </c>
+      <c r="D269" t="n">
+        <v>0</v>
+      </c>
+      <c r="E269" t="n">
+        <v>0</v>
+      </c>
+      <c r="F269" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G269" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H269" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I269" t="n">
+        <v>0</v>
+      </c>
+      <c r="J269" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>TEKFEN.IS</t>
+        </is>
+      </c>
+      <c r="B270" s="1" t="n">
+        <v>45016</v>
+      </c>
+      <c r="C270" t="n">
+        <v>0</v>
+      </c>
+      <c r="D270" t="n">
+        <v>0</v>
+      </c>
+      <c r="E270" t="n">
+        <v>0</v>
+      </c>
+      <c r="F270" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G270" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H270" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I270" t="n">
+        <v>0</v>
+      </c>
+      <c r="J270" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>TEKFEN.IS</t>
+        </is>
+      </c>
+      <c r="B271" s="1" t="n">
+        <v>45199</v>
+      </c>
+      <c r="C271" t="n">
+        <v>0</v>
+      </c>
+      <c r="D271" t="n">
+        <v>0</v>
+      </c>
+      <c r="E271" t="n">
+        <v>0</v>
+      </c>
+      <c r="F271" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G271" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H271" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I271" t="n">
+        <v>0</v>
+      </c>
+      <c r="J271" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>TEKFEN.IS</t>
+        </is>
+      </c>
+      <c r="B272" s="1" t="n">
+        <v>45382</v>
+      </c>
+      <c r="C272" t="n">
+        <v>0</v>
+      </c>
+      <c r="D272" t="n">
+        <v>0</v>
+      </c>
+      <c r="E272" t="n">
+        <v>0</v>
+      </c>
+      <c r="F272" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G272" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H272" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I272" t="n">
+        <v>0</v>
+      </c>
+      <c r="J272" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>TEKFEN.IS</t>
+        </is>
+      </c>
+      <c r="B273" s="1" t="n">
+        <v>45565</v>
+      </c>
+      <c r="C273" t="n">
+        <v>0</v>
+      </c>
+      <c r="D273" t="n">
+        <v>0</v>
+      </c>
+      <c r="E273" t="n">
+        <v>0</v>
+      </c>
+      <c r="F273" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G273" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H273" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I273" t="n">
+        <v>0</v>
+      </c>
+      <c r="J273" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>TEKFEN.IS</t>
+        </is>
+      </c>
+      <c r="B274" s="1" t="n">
+        <v>45747</v>
+      </c>
+      <c r="C274" t="n">
+        <v>0</v>
+      </c>
+      <c r="D274" t="n">
+        <v>0</v>
+      </c>
+      <c r="E274" t="n">
+        <v>0</v>
+      </c>
+      <c r="F274" t="n">
+        <v>108.0379492873263</v>
+      </c>
+      <c r="G274" t="n">
+        <v>7.413588252984848</v>
+      </c>
+      <c r="H274" t="n">
+        <v>0.2106240981789207</v>
+      </c>
+      <c r="I274" t="n">
+        <v>0</v>
+      </c>
+      <c r="J274" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>